<commit_message>
Sound assets and FMOD upload
</commit_message>
<xml_diff>
--- a/documentaion/AssetList.xlsx
+++ b/documentaion/AssetList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\Spring 2021\IGME671_Final_Project\documentaion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2D9FA6D-D23B-42F0-83D3-4C3728EBC577}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA2D050-930F-495D-BC73-CF949475EEE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="1425" windowWidth="21600" windowHeight="11505" xr2:uid="{8AA114FE-D217-4CE7-85D4-1DB41B2A15BF}"/>
+    <workbookView xWindow="26040" yWindow="10185" windowWidth="15480" windowHeight="10335" xr2:uid="{8AA114FE-D217-4CE7-85D4-1DB41B2A15BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Description</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t xml:space="preserve">Get crying noises </t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>White Noise</t>
+  </si>
+  <si>
+    <t>dl from freesound</t>
+  </si>
+  <si>
+    <t>Event Created in FMOD</t>
   </si>
 </sst>
 </file>
@@ -195,7 +207,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +230,11 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -243,11 +260,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -563,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5C35C0-2FF8-4A85-957D-5C9E20467834}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,9 +592,10 @@
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="54.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,8 +605,11 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -598,7 +620,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -609,7 +631,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -619,8 +641,11 @@
       <c r="C4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -630,8 +655,11 @@
       <c r="C5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -641,8 +669,11 @@
       <c r="C6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -652,8 +683,11 @@
       <c r="C7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -663,8 +697,11 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -674,8 +711,11 @@
       <c r="C9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -685,8 +725,11 @@
       <c r="C10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -696,8 +739,11 @@
       <c r="C11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -707,8 +753,11 @@
       <c r="C12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -718,8 +767,11 @@
       <c r="C13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -729,8 +781,11 @@
       <c r="C14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -740,8 +795,11 @@
       <c r="C15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -751,8 +809,11 @@
       <c r="C16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -762,8 +823,26 @@
       <c r="C17" t="s">
         <v>45</v>
       </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final document and build
</commit_message>
<xml_diff>
--- a/documentaion/AssetList.xlsx
+++ b/documentaion/AssetList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\Spring 2021\IGME671_Final_Project\documentaion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA2D050-930F-495D-BC73-CF949475EEE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BFAF87-9E7F-4500-A7B7-2953779CBCC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26040" yWindow="10185" windowWidth="15480" windowHeight="10335" xr2:uid="{8AA114FE-D217-4CE7-85D4-1DB41B2A15BF}"/>
+    <workbookView xWindow="7260" yWindow="4695" windowWidth="19830" windowHeight="12675" xr2:uid="{8AA114FE-D217-4CE7-85D4-1DB41B2A15BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
   <si>
     <t>Description</t>
   </si>
@@ -45,84 +45,9 @@
     <t>Assets Required</t>
   </si>
   <si>
-    <t>Menu Music</t>
-  </si>
-  <si>
-    <t>Play Song</t>
-  </si>
-  <si>
-    <t>Game Lost</t>
-  </si>
-  <si>
-    <t>Footsteps</t>
-  </si>
-  <si>
-    <t>Correct Noise</t>
-  </si>
-  <si>
-    <t>Grab Item</t>
-  </si>
-  <si>
-    <t>Air Conditioner</t>
-  </si>
-  <si>
     <t>Router</t>
   </si>
   <si>
-    <t>Feeding Fish</t>
-  </si>
-  <si>
-    <t>Getting Coffee</t>
-  </si>
-  <si>
-    <t>Water Plants</t>
-  </si>
-  <si>
-    <t>Get Apple</t>
-  </si>
-  <si>
-    <t>Bored Sound</t>
-  </si>
-  <si>
-    <t>Angry Sound</t>
-  </si>
-  <si>
-    <t>Sad Sound</t>
-  </si>
-  <si>
-    <t>Very Sad Sound</t>
-  </si>
-  <si>
-    <t>Problem 1</t>
-  </si>
-  <si>
-    <t>Problem 2</t>
-  </si>
-  <si>
-    <t>Problem 3</t>
-  </si>
-  <si>
-    <t>Problem 4</t>
-  </si>
-  <si>
-    <t>Problem 5</t>
-  </si>
-  <si>
-    <t>Problem 6</t>
-  </si>
-  <si>
-    <t>Emotion 1</t>
-  </si>
-  <si>
-    <t>Emotion 2</t>
-  </si>
-  <si>
-    <t>Emotion 3</t>
-  </si>
-  <si>
-    <t>Emotion 4</t>
-  </si>
-  <si>
     <t>Ambience</t>
   </si>
   <si>
@@ -177,13 +102,70 @@
     <t>Status</t>
   </si>
   <si>
-    <t>White Noise</t>
-  </si>
-  <si>
     <t>dl from freesound</t>
   </si>
   <si>
-    <t>Event Created in FMOD</t>
+    <t>Game_Ambience</t>
+  </si>
+  <si>
+    <t>Keyboard noises, loud talking/crowd noises</t>
+  </si>
+  <si>
+    <t>Mixed, implemented in game</t>
+  </si>
+  <si>
+    <t>Walking</t>
+  </si>
+  <si>
+    <t>White_Noise</t>
+  </si>
+  <si>
+    <t>Game_Over</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Game_Song</t>
+  </si>
+  <si>
+    <t>Emotion</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Bored</t>
+  </si>
+  <si>
+    <t>Angry</t>
+  </si>
+  <si>
+    <t>Sad</t>
+  </si>
+  <si>
+    <t>Very_Sad</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Feed_Fish</t>
+  </si>
+  <si>
+    <t>Pour_Coffee</t>
+  </si>
+  <si>
+    <t>Water_Plants</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Grab_Item</t>
   </si>
 </sst>
 </file>
@@ -581,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5C35C0-2FF8-4A85-957D-5C9E20467834}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,242 +588,265 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:D19">
+    <sortCondition ref="A18:A19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>